<commit_message>
Changes as of 06/03
</commit_message>
<xml_diff>
--- a/InputFiles/CDS/TC04_CDS_phs002305_LibSel-HybridSel_LibLay-PairedEnd_InstMod-Illumina NovaSeq 6000.xlsx
+++ b/InputFiles/CDS/TC04_CDS_phs002305_LibSel-HybridSel_LibLay-PairedEnd_InstMod-Illumina NovaSeq 6000.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation\Sowjanya0528\Commons_Automation\InputFiles\CDS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation\sowjany0601\Commons_Automation\InputFiles\CDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91795C51-27B3-4DDA-A561-470979E62B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8FBD86-86CD-46B8-8333-C66B396BD4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -95,86 +95,6 @@
     (SELECT COUNT(*) FROM Filtered_Participants) AS "Participants",
     (SELECT COUNT(*) FROM Filtered_Samples) AS "Samples",
     (SELECT COUNT(*) FROM Filtered_Files) AS "Files";</t>
-  </si>
-  <si>
-    <t>SELECT
-    f1.file_name AS "File Name",
-    s.study_name AS "Study Name",
-    s.phs_accession AS "Accession",
-    sp.participant_id AS "Participant Id",
-    COALESCE((
-        SELECT
-            REPLACE(GROUP_CONCAT(CASE WHEN rn &lt;= 5 THEN smp.sample_id ELSE NULL END, ', '), ', , ', ', ') ||
-            CASE WHEN MAX(rn) &gt; 5 THEN ', ...' ELSE '' END
-        FROM (
-            SELECT
-                smp.sample_id,
-                ROW_NUMBER() OVER (ORDER BY smp.sample_id) AS rn
-            FROM df_sample smp
-            WHERE smp."participant.study_participant_id" = sp.study_participant_id
-        ) smp
-    ), '') AS "Sample Id",
-    f1.file_type AS "File Type",
-    gi.library_strategy AS "Library Strategy",
-'' AS "Supplementary Files"
-FROM 
-    df_study s
-INNER JOIN 
-    df_participant sp ON sp."study.phs_accession" = s.phs_accession
-INNER JOIN  
-    df_sample smp ON smp."participant.study_participant_id" = sp.study_participant_id
-INNER JOIN 
-    df_file f1 ON f1."sample.sample_id" = smp.sample_id
-INNER JOIN
-    df_genomic_info gi ON gi."file.file_id" = f1.file_id
-INNER JOIN
-    df_diagnosis d ON d."participant.study_participant_id" = sp.study_participant_id
-INNER JOIN
-    df_program p ON p.program_acronym = s."program.program_acronym"
-WHERE 
-s.phs_accession = 'phs002305'
-        AND gi.library_selection = 'Hybrid Selection'
-        AND gi.library_layout = 'Paired-End' 
-        AND gi.instrument_model = 'Illumina NovaSeq 6000'
-GROUP BY
-    f1.file_name,
-    s.study_name,
-    s.phs_accession,
-    sp.participant_id,
-    f1.file_type,
-    gi.library_strategy
-ORDER BY 
-    f1.file_name ASC
---LIMIT 100;</t>
-  </si>
-  <si>
-    <t>WITH Filtered_Files AS (
-    SELECT DISTINCT f.file_id, sp.participant_id
-    FROM df_file f
-    JOIN df_participant sp ON f."participant.study_participant_id" = sp.study_participant_id
-    JOIN df_study s ON sp."study.phs_accession" = s.phs_accession
-    JOIN df_genomic_info gi ON gi."file.file_id" = f.file_id
-    WHERE 
-       s.phs_accession = 'phs002305'
-        AND gi.library_selection = 'Hybrid Selection'
-        AND gi.library_layout = 'Paired-End' 
-        AND gi.instrument_model = 'Illumina NovaSeq 6000'
-),
-Filtered_Participants AS (
-    SELECT DISTINCT participant_id
-    FROM Filtered_Files
-)
-SELECT
-    smp.sample_id AS "Sample ID",
-    sp.participant_id AS "Participant ID",
-    s.study_name AS "Study Name",
-    s.phs_accession AS "Accession"
-FROM df_sample smp
-JOIN df_participant sp ON smp."participant.study_participant_id" = sp.study_participant_id
-JOIN df_study s ON sp."study.phs_accession" = s.phs_accession
-JOIN Filtered_Participants fp ON sp.participant_id = fp.participant_id
-ORDER BY smp.sample_id ASC
---LIMIT 100;</t>
   </si>
   <si>
     <t>WITH Filtered_Participants AS (
@@ -234,7 +154,87 @@
         ELSE sample_list
     END AS Samples
 FROM Sample_Groups
---LIMIT 100;</t>
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>WITH Filtered_Files AS (
+    SELECT DISTINCT f.file_id, sp.participant_id
+    FROM df_file f
+    JOIN df_participant sp ON f."participant.study_participant_id" = sp.study_participant_id
+    JOIN df_study s ON sp."study.phs_accession" = s.phs_accession
+    JOIN df_genomic_info gi ON gi."file.file_id" = f.file_id
+    WHERE 
+       s.phs_accession = 'phs002305'
+        AND gi.library_selection = 'Hybrid Selection'
+        AND gi.library_layout = 'Paired-End' 
+        AND gi.instrument_model = 'Illumina NovaSeq 6000'
+),
+Filtered_Participants AS (
+    SELECT DISTINCT participant_id
+    FROM Filtered_Files
+)
+SELECT
+    smp.sample_id AS "Sample ID",
+    sp.participant_id AS "Participant ID",
+    s.study_name AS "Study Name",
+    s.phs_accession AS "Accession"
+FROM df_sample smp
+JOIN df_participant sp ON smp."participant.study_participant_id" = sp.study_participant_id
+JOIN df_study s ON sp."study.phs_accession" = s.phs_accession
+JOIN Filtered_Participants fp ON sp.participant_id = fp.participant_id
+ORDER BY smp.sample_id ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT
+    f1.file_name AS "File Name",
+    s.study_name AS "Study Name",
+    s.phs_accession AS "Accession",
+    sp.participant_id AS "Participant Id",
+    COALESCE((
+        SELECT
+            REPLACE(GROUP_CONCAT(CASE WHEN rn &lt;= 5 THEN smp.sample_id ELSE NULL END, ', '), ', , ', ', ') ||
+            CASE WHEN MAX(rn) &gt; 5 THEN ', ...' ELSE '' END
+        FROM (
+            SELECT
+                smp.sample_id,
+                ROW_NUMBER() OVER (ORDER BY smp.sample_id) AS rn
+            FROM df_sample smp
+            WHERE smp."participant.study_participant_id" = sp.study_participant_id
+        ) smp
+    ), '') AS "Sample Id",
+    f1.file_type AS "File Type",
+    gi.library_strategy AS "Library Strategy",
+'' AS "Supplementary Files"
+FROM 
+    df_study s
+INNER JOIN 
+    df_participant sp ON sp."study.phs_accession" = s.phs_accession
+INNER JOIN  
+    df_sample smp ON smp."participant.study_participant_id" = sp.study_participant_id
+INNER JOIN 
+    df_file f1 ON f1."sample.sample_id" = smp.sample_id
+INNER JOIN
+    df_genomic_info gi ON gi."file.file_id" = f1.file_id
+INNER JOIN
+    df_diagnosis d ON d."participant.study_participant_id" = sp.study_participant_id
+INNER JOIN
+    df_program p ON p.program_acronym = s."program.program_acronym"
+WHERE 
+s.phs_accession = 'phs002305'
+        AND gi.library_selection = 'Hybrid Selection'
+        AND gi.library_layout = 'Paired-End' 
+        AND gi.instrument_model = 'Illumina NovaSeq 6000'
+GROUP BY
+    f1.file_name,
+    s.study_name,
+    s.phs_accession,
+    sp.participant_id,
+    f1.file_type,
+    gi.library_strategy
+ORDER BY 
+    f1.file_name ASC
+LIMIT 100;</t>
   </si>
 </sst>
 </file>
@@ -626,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +660,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>10</v>
@@ -686,7 +686,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2"/>
     </row>

</xml_diff>